<commit_message>
ajout leçon et exercice sur Flask
</commit_message>
<xml_diff>
--- a/template/horaire.xlsx
+++ b/template/horaire.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/etiennerivard/notes_de_cours/bd2/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3D59B4B-3A9A-0E42-A479-83E26FBD3FEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D96F3B0-DD07-B643-ABC4-3B22C6EA0A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3000" yWindow="1920" windowWidth="27240" windowHeight="16440" xr2:uid="{4696F4E7-E751-AB46-8D30-A385E7EE1466}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="72">
   <si>
     <t>Date</t>
   </si>
@@ -868,6 +868,66 @@
 [Présentation de l'outil drawio](outils/drawio.md)&lt;br/&gt;
 [Convention de nommage MySQL](mysql/convention.md)&lt;br/&gt;
 Exercice 3B - Créer le diagramme de classes du système&lt;br/&gt;</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>Exercice 13 - Flask</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF6796E6"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>exercices/ex13_enonce.md</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF6796E6"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>[Flask](python/flask.md)&lt;br/&gt;Exercice 13</t>
   </si>
 </sst>
 </file>
@@ -1279,8 +1339,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A10D1181-B3CD-EE43-9E3F-518A899CAD6B}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1569,7 +1629,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>9</v>
       </c>
@@ -1579,10 +1639,12 @@
       <c r="C18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D18" t="s">
-        <v>53</v>
-      </c>
-      <c r="E18" s="3"/>
+      <c r="D18" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
@@ -1595,7 +1657,7 @@
         <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="E19" s="3"/>
     </row>

</xml_diff>

<commit_message>
mise à jour horaire 2024
</commit_message>
<xml_diff>
--- a/template/horaire.xlsx
+++ b/template/horaire.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/etiennerivard/notes_de_cours/bd2/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D96F3B0-DD07-B643-ABC4-3B22C6EA0A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF9EF25-5B26-C342-8C97-592AB74AFD5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3000" yWindow="1920" windowWidth="27240" windowHeight="16440" xr2:uid="{4696F4E7-E751-AB46-8D30-A385E7EE1466}"/>
   </bookViews>
@@ -36,99 +36,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
   <si>
     <t>Date</t>
-  </si>
-  <si>
-    <t>2023-08-21</t>
-  </si>
-  <si>
-    <t>2023-08-23</t>
-  </si>
-  <si>
-    <t>2023-08-28</t>
-  </si>
-  <si>
-    <t>2023-08-30</t>
-  </si>
-  <si>
-    <t>2023-09-06</t>
-  </si>
-  <si>
-    <t>2023-09-11</t>
-  </si>
-  <si>
-    <t>2023-09-13</t>
-  </si>
-  <si>
-    <t>2023-09-18</t>
-  </si>
-  <si>
-    <t>2023-09-20</t>
-  </si>
-  <si>
-    <t>2023-09-25</t>
-  </si>
-  <si>
-    <t>2023-09-27</t>
-  </si>
-  <si>
-    <t>2023-10-02</t>
-  </si>
-  <si>
-    <t>2023-10-16</t>
-  </si>
-  <si>
-    <t>2023-10-18</t>
-  </si>
-  <si>
-    <t>2023-10-23</t>
-  </si>
-  <si>
-    <t>2023-10-25</t>
-  </si>
-  <si>
-    <t>2023-10-30</t>
-  </si>
-  <si>
-    <t>2023-11-01</t>
-  </si>
-  <si>
-    <t>2023-11-06</t>
-  </si>
-  <si>
-    <t>2023-11-09</t>
-  </si>
-  <si>
-    <t>2023-11-13</t>
-  </si>
-  <si>
-    <t>2023-11-15</t>
-  </si>
-  <si>
-    <t>2023-11-20</t>
-  </si>
-  <si>
-    <t>2023-11-22</t>
-  </si>
-  <si>
-    <t>2023-11-27</t>
-  </si>
-  <si>
-    <t>2023-11-29</t>
-  </si>
-  <si>
-    <t>2023-12-04</t>
-  </si>
-  <si>
-    <t>2023-12-06</t>
-  </si>
-  <si>
-    <t>2023-12-11</t>
-  </si>
-  <si>
-    <t>2023-12-15</t>
   </si>
   <si>
     <t>Cours</t>
@@ -975,18 +885,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDCE6F1"/>
-        <bgColor rgb="FFDCE6F1"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -1001,21 +905,17 @@
       <left/>
       <right/>
       <top style="thin">
-        <color rgb="FF95B3D7"/>
+        <color theme="5"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF95B3D7"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1023,6 +923,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1339,8 +1240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A10D1181-B3CD-EE43-9E3F-518A899CAD6B}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1351,19 +1252,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>33</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1373,14 +1274,14 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>1</v>
+      <c r="C2" s="4">
+        <v>45525.552083333336</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>55</v>
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="119" x14ac:dyDescent="0.2">
@@ -1390,14 +1291,14 @@
       <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>56</v>
+      <c r="C3" s="4">
+        <v>45530.34375</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="85" x14ac:dyDescent="0.2">
@@ -1407,14 +1308,14 @@
       <c r="B4">
         <v>3</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>57</v>
+      <c r="C4" s="4">
+        <v>45532.552083333336</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="51" x14ac:dyDescent="0.2">
@@ -1424,14 +1325,14 @@
       <c r="B5">
         <v>4</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>58</v>
+      <c r="C5" s="4">
+        <v>45540.34375</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -1441,14 +1342,14 @@
       <c r="B6">
         <v>5</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>59</v>
+      <c r="C6" s="4">
+        <v>45544.34375</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1458,14 +1359,14 @@
       <c r="B7">
         <v>6</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>6</v>
+      <c r="C7" s="4">
+        <v>45546.552083333336</v>
       </c>
       <c r="D7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>60</v>
+        <v>9</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -1475,11 +1376,11 @@
       <c r="B8">
         <v>7</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>7</v>
+      <c r="C8" s="4">
+        <v>45551.34375</v>
       </c>
       <c r="D8" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="68" x14ac:dyDescent="0.2">
@@ -1489,14 +1390,14 @@
       <c r="B9">
         <v>8</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>61</v>
+      <c r="C9" s="4">
+        <v>45553.552083333336</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="85" x14ac:dyDescent="0.2">
@@ -1506,14 +1407,14 @@
       <c r="B10">
         <v>9</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>67</v>
+      <c r="C10" s="4">
+        <v>45558.34375</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -1523,14 +1424,14 @@
       <c r="B11">
         <v>10</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>10</v>
+      <c r="C11" s="4">
+        <v>45560.552083333336</v>
       </c>
       <c r="D11" t="s">
-        <v>66</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>67</v>
+        <v>36</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -1540,11 +1441,11 @@
       <c r="B12">
         <v>11</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>11</v>
+      <c r="C12" s="4">
+        <v>45565.34375</v>
       </c>
       <c r="D12" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -1554,11 +1455,11 @@
       <c r="B13">
         <v>12</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>12</v>
+      <c r="C13" s="4">
+        <v>45567.552083333336</v>
       </c>
       <c r="D13" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="51" x14ac:dyDescent="0.2">
@@ -1568,14 +1469,14 @@
       <c r="B14">
         <v>13</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>37</v>
+      <c r="C14" s="4">
+        <v>45572.34375</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="68" x14ac:dyDescent="0.2">
@@ -1585,14 +1486,14 @@
       <c r="B15">
         <v>14</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>36</v>
+      <c r="C15" s="4">
+        <v>45574.552083333336</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="51" x14ac:dyDescent="0.2">
@@ -1602,14 +1503,14 @@
       <c r="B16">
         <v>15</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>35</v>
+      <c r="C16" s="4">
+        <v>45586.34375</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -1619,14 +1520,14 @@
       <c r="B17">
         <v>16</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>16</v>
+      <c r="C17" s="4">
+        <v>45588.552083333336</v>
       </c>
       <c r="D17" t="s">
-        <v>44</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>35</v>
+        <v>14</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -1636,14 +1537,14 @@
       <c r="B18">
         <v>17</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>70</v>
+      <c r="C18" s="4">
+        <v>45593.34375</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -1653,13 +1554,13 @@
       <c r="B19">
         <v>18</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>18</v>
+      <c r="C19" s="4">
+        <v>45595.552083333336</v>
       </c>
       <c r="D19" t="s">
-        <v>53</v>
-      </c>
-      <c r="E19" s="3"/>
+        <v>23</v>
+      </c>
+      <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
@@ -1668,13 +1569,13 @@
       <c r="B20">
         <v>19</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>19</v>
+      <c r="C20" s="4">
+        <v>45600.34375</v>
       </c>
       <c r="D20" t="s">
-        <v>45</v>
-      </c>
-      <c r="E20" s="3"/>
+        <v>15</v>
+      </c>
+      <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
@@ -1683,11 +1584,11 @@
       <c r="B21">
         <v>20</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>20</v>
+      <c r="C21" s="4">
+        <v>45604.552083333336</v>
       </c>
       <c r="D21" t="s">
-        <v>45</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -1697,11 +1598,11 @@
       <c r="B22">
         <v>21</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>21</v>
+      <c r="C22" s="4">
+        <v>45607.34375</v>
       </c>
       <c r="D22" t="s">
-        <v>45</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -1711,11 +1612,11 @@
       <c r="B23">
         <v>22</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>22</v>
+      <c r="C23" s="4">
+        <v>45609.552083333336</v>
       </c>
       <c r="D23" t="s">
-        <v>45</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -1725,11 +1626,11 @@
       <c r="B24">
         <v>23</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>23</v>
+      <c r="C24" s="4">
+        <v>45614.34375</v>
       </c>
       <c r="D24" t="s">
-        <v>45</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -1739,11 +1640,11 @@
       <c r="B25">
         <v>24</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>24</v>
+      <c r="C25" s="4">
+        <v>45616.552083333336</v>
       </c>
       <c r="D25" t="s">
-        <v>45</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -1753,11 +1654,11 @@
       <c r="B26">
         <v>25</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>25</v>
+      <c r="C26" s="4">
+        <v>45621.34375</v>
       </c>
       <c r="D26" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -1767,11 +1668,11 @@
       <c r="B27">
         <v>26</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>26</v>
+      <c r="C27" s="4">
+        <v>45623.552083333336</v>
       </c>
       <c r="D27" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -1781,11 +1682,11 @@
       <c r="B28">
         <v>27</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>27</v>
+      <c r="C28" s="4">
+        <v>45628.34375</v>
       </c>
       <c r="D28" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -1795,11 +1696,11 @@
       <c r="B29">
         <v>28</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>28</v>
+      <c r="C29" s="4">
+        <v>45630.552083333336</v>
       </c>
       <c r="D29" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -1809,11 +1710,11 @@
       <c r="B30">
         <v>29</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>29</v>
+      <c r="C30" s="4">
+        <v>45635.34375</v>
       </c>
       <c r="D30" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -1823,11 +1724,11 @@
       <c r="B31">
         <v>30</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>30</v>
+      <c r="C31" s="4">
+        <v>45637.552083333336</v>
       </c>
       <c r="D31" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ajout dotenv et correction horaire
</commit_message>
<xml_diff>
--- a/template/horaire.xlsx
+++ b/template/horaire.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/etiennerivard/notes_de_cours/bd2/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E323FB9-78CE-9840-AD42-40AE22E8511F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{256AF946-0D92-204F-9D6B-0BD0060807D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3000" yWindow="1920" windowWidth="27240" windowHeight="16440" xr2:uid="{4696F4E7-E751-AB46-8D30-A385E7EE1466}"/>
   </bookViews>
@@ -756,11 +756,6 @@
     </r>
   </si>
   <si>
-    <t>Retour sur l'examen 1&lt;br/&gt;
-Retour sur les curseurs et la gestion d'erreurs, les jointures et union&lt;br/&gt;
-Exercice 10</t>
-  </si>
-  <si>
     <t>Exercice 3 - Le système de stationnement du Cégep (partie A)&lt;br/&gt;
 [Théorie sur les diagrammes de classes](modelisation/classes.md)&lt;br/&gt;
 [Présentation de l'outil drawio](outils/drawio.md)&lt;br/&gt;
@@ -828,12 +823,6 @@
     <t>[Flask](python/flask.md)&lt;br/&gt;Exercice 13</t>
   </si>
   <si>
-    <t>[Installation de Python](python/installation.md)&lt;br/&gt;
-[Utilisation du connecteur MySQL](python/mysql_connector.md)&lt;br/&gt;
-[PyDoc](python/documentation.md)&lt;br/&gt;
-Exercice 12</t>
-  </si>
-  <si>
     <t>[Transactions](mysql/transactions.md)&lt;br/&gt;
 [Procédures stockées](mysql/procedures.md)&lt;br/&gt;
 [Gestion des erreurs](mysql/gestion_erreurs.md)&lt;br/&gt;
@@ -899,6 +888,19 @@
       </rPr>
       <t>)</t>
     </r>
+  </si>
+  <si>
+    <t>Retour sur l'examen 1&lt;br/&gt;
+Exercice 10</t>
+  </si>
+  <si>
+    <t>[Installation de Python](python/installation.md)&lt;br/&gt;
+[Environnements virtuels](python/venv.md)&lt;br/&gt;
+[PIP](python/pip.md)&lt;br/&gt;
+[DotEnv](python/dotenv.md)&lt;br/&gt;
+[Utilisation du connecteur MySQL](python/mysql_connector.md)&lt;br/&gt;
+[PyDoc](python/documentation.md)&lt;br/&gt;
+Exercice 12</t>
   </si>
 </sst>
 </file>
@@ -1301,8 +1303,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A10D1181-B3CD-EE43-9E3F-518A899CAD6B}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1373,7 +1375,7 @@
         <v>45532.552083333336</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>26</v>
@@ -1472,7 +1474,7 @@
         <v>45558.34375</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>35</v>
@@ -1509,7 +1511,7 @@
         <v>10</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -1526,7 +1528,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>7</v>
       </c>
@@ -1537,7 +1539,7 @@
         <v>45572.34375</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>7</v>
@@ -1560,7 +1562,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="119" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>8</v>
       </c>
@@ -1571,7 +1573,7 @@
         <v>45586.34375</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>5</v>
@@ -1605,10 +1607,10 @@
         <v>45593.34375</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -1764,7 +1766,7 @@
         <v>45630.552083333336</v>
       </c>
       <c r="D29" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>